<commit_message>
4/12/21 Changes - Context Passing of Log variable
Fixed context passing to pressure sensor log variable.
</commit_message>
<xml_diff>
--- a/Controls/VoltageSensorCalibration.xlsx
+++ b/Controls/VoltageSensorCalibration.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Spring_2021_Semester\ENGR340\CAES_Controls\CAES_Controls\Controls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C44DE20-E9FA-4CD7-A848-9A137D358770}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA362322-7999-4F1D-8BA3-6794D6C5A9EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E60A4FC2-820A-41B4-8238-FB3260EA5069}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E60A4FC2-820A-41B4-8238-FB3260EA5069}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VoltageCalibration" sheetId="1" r:id="rId1"/>
+    <sheet name="CurrentCalibration" sheetId="2" r:id="rId2"/>
+    <sheet name="PressureCalibration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -244,42 +256,60 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>VoltageCalibration!$C$1:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>811</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:f>VoltageCalibration!$B$1:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>613</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>408</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>820</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>203</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,7 +508,925 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CurrentCalibration!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CurrentCalibration!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>542</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CurrentCalibration!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD10-4CB6-8B09-77E22FD3B8A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="396478632"/>
+        <c:axId val="396478960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="396478632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396478960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="396478960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396478632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PressureCalibration!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PressureCalibration!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PressureCalibration!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1AE8-4280-80BE-31B901372C9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="496794896"/>
+        <c:axId val="496795880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="496794896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496795880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="496795880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496794896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1034,20 +1982,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1055,6 +3035,88 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F31E6A5-5AA6-4244-9CF3-4F3CCBD40DDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D85B88-7773-4E2B-AEE7-C7F5AD27631B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29621E2-D63E-4633-9355-A37CE5B6B38F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A001E1B7-D12B-4B10-80F7-8B437BC5B094}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,7 +3450,7 @@
         <v>15</v>
       </c>
       <c r="C1">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1399,7 +3461,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1407,7 +3469,7 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>820</v>
+        <v>811</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1415,7 +3477,249 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>203</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F1B0D4-019B-40F1-80DA-DD0D8AA231D5}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.05</v>
+      </c>
+      <c r="B3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.25</v>
+      </c>
+      <c r="B5">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.3</v>
+      </c>
+      <c r="B6">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.45</v>
+      </c>
+      <c r="B7">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.65</v>
+      </c>
+      <c r="B9">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.8</v>
+      </c>
+      <c r="B10">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF94ABF6-1270-46E2-B342-C280764F77FC}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>105</v>
+      </c>
+      <c r="B2">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>